<commit_message>
[UPD] Added new data
</commit_message>
<xml_diff>
--- a/data/monthly_data_max.xlsx
+++ b/data/monthly_data_max.xlsx
@@ -688,7 +688,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>2025</t>
+          <t>2024</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -697,11 +697,11 @@
         </is>
       </c>
       <c r="P2" t="n">
-        <v>7.2</v>
+        <v>4.1</v>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>2025</t>
+          <t>2024</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
@@ -710,11 +710,11 @@
         </is>
       </c>
       <c r="S2" t="n">
-        <v>13.39805720899471</v>
+        <v>12.60752813494749</v>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>2025</t>
+          <t>2024</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
@@ -723,11 +723,11 @@
         </is>
       </c>
       <c r="V2" t="n">
-        <v>18.55833333333333</v>
+        <v>18.00322580645161</v>
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>2025</t>
+          <t>2024</t>
         </is>
       </c>
       <c r="X2" t="inlineStr">
@@ -736,7 +736,7 @@
         </is>
       </c>
       <c r="Y2" t="n">
-        <v>9.708333333333334</v>
+        <v>8.480645161290322</v>
       </c>
       <c r="Z2" t="inlineStr">
         <is>
@@ -753,7 +753,7 @@
       </c>
       <c r="AC2" t="inlineStr">
         <is>
-          <t>2025</t>
+          <t>2024</t>
         </is>
       </c>
       <c r="AD2" t="inlineStr">
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="AE2" t="n">
-        <v>9.15324074074074</v>
+        <v>8.525690214803117</v>
       </c>
       <c r="AF2" t="inlineStr">
         <is>

</xml_diff>